<commit_message>
minor change a number was a bit wrong
</commit_message>
<xml_diff>
--- a/Lab2/Part1/SensorCalibrationData.xlsx
+++ b/Lab2/Part1/SensorCalibrationData.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22416"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22624"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="960" yWindow="560" windowWidth="38400" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="7200" yWindow="80" windowWidth="29220" windowHeight="18920" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -234,37 +234,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>3.64</c:v>
+                  <c:v>3.49</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.6</c:v>
+                  <c:v>4.45</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.07</c:v>
+                  <c:v>4.92</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.5</c:v>
+                  <c:v>5.35</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.55</c:v>
+                  <c:v>5.399999999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.0</c:v>
+                  <c:v>5.85</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.5</c:v>
+                  <c:v>6.35</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7.0</c:v>
+                  <c:v>6.85</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7.45</c:v>
+                  <c:v>7.3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>7.93</c:v>
+                  <c:v>7.78</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9.36</c:v>
+                  <c:v>9.21</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -276,7 +276,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.0101538461538462</c:v>
+                  <c:v>0.0103937007874016</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.0116</c:v>
@@ -321,11 +321,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2137253144"/>
-        <c:axId val="-2137278600"/>
+        <c:axId val="2143861000"/>
+        <c:axId val="2143866568"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2137253144"/>
+        <c:axId val="2143861000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -354,12 +354,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2137278600"/>
+        <c:crossAx val="2143866568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2137278600"/>
+        <c:axId val="2143866568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -394,7 +394,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2137253144"/>
+        <c:crossAx val="2143861000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -512,7 +512,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.0101538461538462</c:v>
+                  <c:v>0.0103937007874016</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.0116</c:v>
@@ -557,11 +557,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2133288648"/>
-        <c:axId val="-2133000104"/>
+        <c:axId val="2143898232"/>
+        <c:axId val="2143903944"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2133288648"/>
+        <c:axId val="2143898232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -595,12 +595,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2133000104"/>
+        <c:crossAx val="2143903944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2133000104"/>
+        <c:axId val="2143903944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -635,7 +635,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2133288648"/>
+        <c:crossAx val="2143898232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1041,8 +1041,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1100,7 +1100,8 @@
         <v>14</v>
       </c>
       <c r="B8">
-        <v>6.5</v>
+        <f>12.7 / 2</f>
+        <v>6.35</v>
       </c>
       <c r="D8" t="s">
         <v>15</v>
@@ -1163,14 +1164,14 @@
       </c>
       <c r="C14">
         <f>B14+$B$8</f>
-        <v>3.64</v>
+        <v>3.4899999999999998</v>
       </c>
       <c r="D14">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="E14">
         <f>(D14 - $B$10) / $B$8</f>
-        <v>1.0153846153846154E-2</v>
+        <v>1.0393700787401577E-2</v>
       </c>
       <c r="F14">
         <f>B14-121+129.5+1.23-12.7/2</f>
@@ -1184,7 +1185,7 @@
       </c>
       <c r="C15">
         <f>B15+$B$8</f>
-        <v>4.5999999999999996</v>
+        <v>4.4499999999999993</v>
       </c>
       <c r="D15">
         <v>0.12</v>
@@ -1194,7 +1195,7 @@
         <v>1.1599999999999999E-2</v>
       </c>
       <c r="F15">
-        <f t="shared" ref="F15:F24" si="0">B15-121+129.5+1.23-12.7/2</f>
+        <f>B15-121+129.5+1.23-12.7/2</f>
         <v>1.4799999999999951</v>
       </c>
     </row>
@@ -1203,22 +1204,22 @@
         <v>-1</v>
       </c>
       <c r="B16">
-        <f t="shared" ref="B16" si="1">A16*$B$7</f>
+        <f t="shared" ref="B16" si="0">A16*$B$7</f>
         <v>-1.43</v>
       </c>
       <c r="C16">
-        <f t="shared" ref="C16" si="2">B16+$B$8</f>
-        <v>5.07</v>
+        <f t="shared" ref="C16" si="1">B16+$B$8</f>
+        <v>4.92</v>
       </c>
       <c r="D16">
         <v>1.1200000000000001</v>
       </c>
       <c r="E16">
-        <f t="shared" ref="E15:E24" si="3">(D16 - $B$10) / $B$9</f>
+        <f t="shared" ref="E16:E24" si="2">(D16 - $B$10) / $B$9</f>
         <v>0.1116</v>
       </c>
       <c r="F16">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="F15:F24" si="3">B16-121+129.5+1.23-12.7/2</f>
         <v>1.949999999999994</v>
       </c>
     </row>
@@ -1227,18 +1228,18 @@
         <v>-1</v>
       </c>
       <c r="C17">
-        <f>B17+$B$8</f>
-        <v>5.5</v>
+        <f t="shared" ref="C17:C24" si="4">B17+$B$8</f>
+        <v>5.35</v>
       </c>
       <c r="D17">
         <v>1.3</v>
       </c>
       <c r="E17">
+        <f t="shared" si="2"/>
+        <v>0.12959999999999999</v>
+      </c>
+      <c r="F17">
         <f t="shared" si="3"/>
-        <v>0.12959999999999999</v>
-      </c>
-      <c r="F17">
-        <f t="shared" si="0"/>
         <v>2.3800000000000008</v>
       </c>
     </row>
@@ -1247,18 +1248,18 @@
         <v>-0.95</v>
       </c>
       <c r="C18">
-        <f>B18+$B$8</f>
-        <v>5.55</v>
+        <f t="shared" si="4"/>
+        <v>5.3999999999999995</v>
       </c>
       <c r="D18">
         <v>2.17</v>
       </c>
       <c r="E18">
+        <f t="shared" si="2"/>
+        <v>0.21659999999999999</v>
+      </c>
+      <c r="F18">
         <f t="shared" si="3"/>
-        <v>0.21659999999999999</v>
-      </c>
-      <c r="F18">
-        <f t="shared" si="0"/>
         <v>2.4299999999999979</v>
       </c>
     </row>
@@ -1267,18 +1268,18 @@
         <v>-0.5</v>
       </c>
       <c r="C19">
-        <f>B19+$B$8</f>
-        <v>6</v>
+        <f t="shared" si="4"/>
+        <v>5.85</v>
       </c>
       <c r="D19">
         <v>4.38</v>
       </c>
       <c r="E19">
+        <f t="shared" si="2"/>
+        <v>0.43760000000000004</v>
+      </c>
+      <c r="F19">
         <f t="shared" si="3"/>
-        <v>0.43760000000000004</v>
-      </c>
-      <c r="F19">
-        <f t="shared" si="0"/>
         <v>2.8800000000000008</v>
       </c>
     </row>
@@ -1291,18 +1292,18 @@
         <v>0</v>
       </c>
       <c r="C20">
-        <f>B20+$B$8</f>
-        <v>6.5</v>
+        <f t="shared" si="4"/>
+        <v>6.35</v>
       </c>
       <c r="D20">
         <v>7.01</v>
       </c>
       <c r="E20">
+        <f t="shared" si="2"/>
+        <v>0.7006</v>
+      </c>
+      <c r="F20">
         <f t="shared" si="3"/>
-        <v>0.7006</v>
-      </c>
-      <c r="F20">
-        <f t="shared" si="0"/>
         <v>3.3800000000000008</v>
       </c>
     </row>
@@ -1311,18 +1312,18 @@
         <v>0.5</v>
       </c>
       <c r="C21">
-        <f>B21+$B$8</f>
-        <v>7</v>
+        <f t="shared" si="4"/>
+        <v>6.85</v>
       </c>
       <c r="D21">
         <v>8.15</v>
       </c>
       <c r="E21">
+        <f t="shared" si="2"/>
+        <v>0.8146000000000001</v>
+      </c>
+      <c r="F21">
         <f t="shared" si="3"/>
-        <v>0.8146000000000001</v>
-      </c>
-      <c r="F21">
-        <f t="shared" si="0"/>
         <v>3.8800000000000008</v>
       </c>
     </row>
@@ -1331,18 +1332,18 @@
         <v>0.95</v>
       </c>
       <c r="C22">
-        <f>B22+$B$8</f>
-        <v>7.45</v>
+        <f t="shared" si="4"/>
+        <v>7.3</v>
       </c>
       <c r="D22">
         <v>9.77</v>
       </c>
       <c r="E22">
+        <f t="shared" si="2"/>
+        <v>0.97660000000000002</v>
+      </c>
+      <c r="F22">
         <f t="shared" si="3"/>
-        <v>0.97660000000000002</v>
-      </c>
-      <c r="F22">
-        <f t="shared" si="0"/>
         <v>4.3300000000000036</v>
       </c>
     </row>
@@ -1355,18 +1356,18 @@
         <v>1.43</v>
       </c>
       <c r="C23">
-        <f>B23+$B$8</f>
-        <v>7.93</v>
+        <f t="shared" si="4"/>
+        <v>7.7799999999999994</v>
       </c>
       <c r="D23">
         <v>9.9499999999999993</v>
       </c>
       <c r="E23">
+        <f t="shared" si="2"/>
+        <v>0.99459999999999993</v>
+      </c>
+      <c r="F23">
         <f t="shared" si="3"/>
-        <v>0.99459999999999993</v>
-      </c>
-      <c r="F23">
-        <f t="shared" si="0"/>
         <v>4.8100000000000076</v>
       </c>
     </row>
@@ -1379,18 +1380,18 @@
         <v>2.86</v>
       </c>
       <c r="C24">
-        <f>B24+$B$8</f>
-        <v>9.36</v>
+        <f t="shared" si="4"/>
+        <v>9.2099999999999991</v>
       </c>
       <c r="D24">
         <v>9.9600000000000009</v>
       </c>
       <c r="E24">
+        <f t="shared" si="2"/>
+        <v>0.99560000000000015</v>
+      </c>
+      <c r="F24">
         <f t="shared" si="3"/>
-        <v>0.99560000000000015</v>
-      </c>
-      <c r="F24">
-        <f t="shared" si="0"/>
         <v>6.24</v>
       </c>
     </row>

</xml_diff>